<commit_message>
more exploration in sklearn
Trying 3 models at once to select right model for the task
</commit_message>
<xml_diff>
--- a/sklearn/sklearn_library.xlsx
+++ b/sklearn/sklearn_library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rostb\Desktop\personal\ML\sklearn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744999E4-7C77-4542-A745-0634DBCD5424}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4C8C6A-DAF8-4FBD-ADC7-78C05C7330C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{EAEB17A8-21EB-4FA6-9037-43A9287A3966}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{EAEB17A8-21EB-4FA6-9037-43A9287A3966}"/>
   </bookViews>
   <sheets>
     <sheet name="cheat sheet" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="regression" sheetId="3" r:id="rId3"/>
     <sheet name="clustering" sheetId="4" r:id="rId4"/>
     <sheet name="dimensionality reduction" sheetId="5" r:id="rId5"/>
+    <sheet name="Tips" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
   <si>
     <t>Kneigbors classifier</t>
   </si>
@@ -178,6 +179,39 @@
   </si>
   <si>
     <t>Links to overview \ Parent class</t>
+  </si>
+  <si>
+    <t>backward \forward attribute selection</t>
+  </si>
+  <si>
+    <t>start from 1 column to train the system and then add more or vise versa</t>
+  </si>
+  <si>
+    <t>Correlation analysis</t>
+  </si>
+  <si>
+    <t>if two or more columns are corelated, for example for big houses land and size of the houses are always bigger than for small houses we don't need to keep land size and house size columns</t>
+  </si>
+  <si>
+    <t>Datasets</t>
+  </si>
+  <si>
+    <t>https://archive.ics.uci.edu/ml/datasets.php</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/datasets</t>
+  </si>
+  <si>
+    <t>Balanced Datframe</t>
+  </si>
+  <si>
+    <t>when target column have similar numbers of 1 and 0</t>
+  </si>
+  <si>
+    <t>EDA - explarotatry Data analysis</t>
+  </si>
+  <si>
+    <t>learn your data: shape(), dtypes, isna().sum(), describe(), df.["target"].value_counts(), corr()</t>
   </si>
 </sst>
 </file>
@@ -244,11 +278,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -630,7 +673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C2667B-FCAB-474C-AF00-DD00E7D43E60}">
   <dimension ref="B2:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -925,4 +968,72 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0512D809-EF10-4C18-83E7-93B989213090}">
+  <dimension ref="B2:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="32.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="90.33203125" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C5" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{C2AA5389-CEF7-479C-97C9-01C85BB6B9D5}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{B2EEF6F0-F604-40A8-BE81-A5443D11A477}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>